<commit_message>
Adding more food items, changes in the amounts in the recipe templates to test scenarios, etc
</commit_message>
<xml_diff>
--- a/data/impacts/impacts_recipe_1.xlsx
+++ b/data/impacts/impacts_recipe_1.xlsx
@@ -440,12 +440,12 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>10.8002438</v>
+        <v>9.749285</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2.4976764</v>
+        <v>2.367085</v>
       </c>
     </row>
     <row r="4">
@@ -455,7 +455,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7.4475798</v>
+        <v>7.402089999999999</v>
       </c>
     </row>
     <row r="6">
@@ -465,47 +465,47 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>18.9666722</v>
+        <v>18.63214</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.610411</v>
+        <v>0.590395</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.2697032</v>
+        <v>0.17663</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.2001236</v>
+        <v>0.129185</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.1130746</v>
+        <v>0.08722000000000001</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.09549330800000001</v>
+        <v>0.09084095</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.089938224</v>
+        <v>0.08669285</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>908.8172</v>
+        <v>788.7049999999999</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>25209.5044</v>
+        <v>18284.165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>